<commit_message>
Basic UI classes finished
</commit_message>
<xml_diff>
--- a/doc/JournalDeBord.xlsx
+++ b/doc/JournalDeBord.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$C$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$C$41</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Nom, Prénom</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Mise en place de Github</t>
+  </si>
+  <si>
+    <t>Remarques</t>
+  </si>
+  <si>
+    <t>Création d'images bitmap pour l'interface</t>
   </si>
 </sst>
 </file>
@@ -126,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -257,11 +263,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -276,8 +293,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -287,6 +302,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,10 +592,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +603,7 @@
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -604,318 +626,367 @@
       <c r="C3" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>43592</v>
       </c>
-      <c r="B4" s="12"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="9"/>
+      <c r="D4" s="18"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="16">
         <v>1.5</v>
       </c>
+      <c r="D5" s="13"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="16">
         <v>0.5</v>
       </c>
+      <c r="D6" s="14"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="16">
         <v>2</v>
       </c>
+      <c r="D7" s="14"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="16">
         <v>1</v>
       </c>
+      <c r="D8" s="14"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="16">
         <v>1.5</v>
       </c>
+      <c r="D9" s="14"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>43593</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="16">
         <v>3</v>
       </c>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="16">
         <v>0.5</v>
       </c>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="16">
         <v>0.5</v>
       </c>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="16">
         <v>0.5</v>
       </c>
+      <c r="D14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="16">
         <v>0.5</v>
       </c>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="14"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>43594</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="10"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="11"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="16">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="14"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="16">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="14"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>43595</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="10"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="11"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="16">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="14"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="16">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>43599</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="11"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="14"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="16">
+        <v>3</v>
+      </c>
+      <c r="D27" s="14"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="D28" s="14"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="14"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
         <v>43600</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="10"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+      <c r="B30" s="11"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="14"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
         <v>43601</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="10"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
+      <c r="B31" s="11"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="14"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
         <v>43602</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="10"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
+      <c r="B32" s="11"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="14"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
         <v>43606</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="10"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+      <c r="B33" s="11"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="14"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
         <v>43607</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="10"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
+      <c r="B34" s="11"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="14"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
         <v>43608</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="10"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
+      <c r="B35" s="11"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="14"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
         <v>43609</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="10"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
+      <c r="B36" s="11"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="14"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
         <v>43613</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="10"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
+      <c r="B37" s="11"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="14"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
         <v>43614</v>
       </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="10"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="7">
+      <c r="B38" s="11"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="14"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
         <v>43620</v>
       </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="10"/>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="8">
+      <c r="B39" s="11"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="14"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="8">
         <v>43621</v>
       </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="11"/>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="B40" s="12"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="15"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="3">
-        <f>SUM(C4:C39)</f>
-        <v>24.5</v>
+      <c r="C41" s="3">
+        <f>SUM(C4:C40)</f>
+        <v>27.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="79" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created XBM images and added them to the code
</commit_message>
<xml_diff>
--- a/doc/JournalDeBord.xlsx
+++ b/doc/JournalDeBord.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$C$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$C$42</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Nom, Prénom</t>
   </si>
@@ -108,7 +108,10 @@
     <t>Remarques</t>
   </si>
   <si>
-    <t>Création d'images bitmap pour l'interface</t>
+    <t>Création d'images bitmap pour l'interface et intégration dans le code</t>
+  </si>
+  <si>
+    <t>Lecture de documentation sur les événements tkinter</t>
   </si>
 </sst>
 </file>
@@ -592,10 +595,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,20 +885,24 @@
       <c r="B29" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="16"/>
+      <c r="C29" s="16">
+        <v>1</v>
+      </c>
       <c r="D29" s="14"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
-        <v>43600</v>
-      </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="16"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="16">
+        <v>0.5</v>
+      </c>
       <c r="D30" s="14"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
-        <v>43601</v>
+        <v>43600</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="16"/>
@@ -903,7 +910,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
-        <v>43602</v>
+        <v>43601</v>
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="16"/>
@@ -911,7 +918,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
-        <v>43606</v>
+        <v>43602</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="16"/>
@@ -919,7 +926,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
-        <v>43607</v>
+        <v>43606</v>
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="16"/>
@@ -927,7 +934,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>43608</v>
+        <v>43607</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="16"/>
@@ -935,7 +942,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
-        <v>43609</v>
+        <v>43608</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="16"/>
@@ -943,7 +950,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
-        <v>43613</v>
+        <v>43609</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="16"/>
@@ -951,7 +958,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
-        <v>43614</v>
+        <v>43613</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="16"/>
@@ -959,30 +966,38 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
-        <v>43620</v>
+        <v>43614</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="16"/>
       <c r="D39" s="14"/>
     </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="8">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <v>43620</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="14"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="8">
         <v>43621</v>
       </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="15"/>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="B41" s="12"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="15"/>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="3">
-        <f>SUM(C4:C40)</f>
-        <v>27.5</v>
+      <c r="C42" s="3">
+        <f>SUM(C4:C41)</f>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented piloting through GUI buttons
</commit_message>
<xml_diff>
--- a/doc/JournalDeBord.xlsx
+++ b/doc/JournalDeBord.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$C$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$C$48</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Nom, Prénom</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Temps (h)</t>
   </si>
   <si>
-    <t>Mise à journ de la planification initiale et du journal de bord</t>
-  </si>
-  <si>
     <t>Mise en place du contrôle de version (Git)</t>
   </si>
   <si>
@@ -112,6 +109,42 @@
   </si>
   <si>
     <t>Lecture de documentation sur les événements tkinter</t>
+  </si>
+  <si>
+    <t>Implémentation du contrôle du robot par l'interface graphique</t>
+  </si>
+  <si>
+    <t>Pour le backup des fichiers et consultation externe</t>
+  </si>
+  <si>
+    <t>Premier jet de l'interface terminé</t>
+  </si>
+  <si>
+    <t>Modification du diagramme UML</t>
+  </si>
+  <si>
+    <t>Inspection du matériel et rediscussion du cahier des charges avec M.Hurni</t>
+  </si>
+  <si>
+    <t>Mise à jour de la planification initiale et du journal de bord</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon ordinateur plantait lorsque j'essayais de me connecter au wifi avec la clé USB. J'ai donc dû travailler sur mon ordinateur personnel </t>
+  </si>
+  <si>
+    <t>Gestion de problème d'infrastructure</t>
+  </si>
+  <si>
+    <t>Implémentation du contrôle par l'interface graphique</t>
+  </si>
+  <si>
+    <t>L'utilisation des subprocess de python a entrainé un certain nombre de contraintes avec lesquelles il a fallut composer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> La technique utilisée actuellement, bien que fonctionnelle, entraîne une latence conséquente dans le pilotage. Il est possible que je doive recourir à une librairie externe pour améliorer cela</t>
   </si>
 </sst>
 </file>
@@ -281,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -305,13 +338,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,10 +635,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +646,7 @@
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="4" max="4" width="58.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -629,8 +669,8 @@
       <c r="C3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>27</v>
+      <c r="D3" s="15" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -639,7 +679,7 @@
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="9"/>
-      <c r="D4" s="18"/>
+      <c r="D4" s="10"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -647,10 +687,10 @@
       <c r="B5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="13">
         <v>1.5</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="16"/>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -658,10 +698,10 @@
       <c r="B6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="13">
         <v>0.5</v>
       </c>
-      <c r="D6" s="14"/>
+      <c r="D6" s="17"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
@@ -670,10 +710,10 @@
       <c r="B7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="13">
         <v>2</v>
       </c>
-      <c r="D7" s="14"/>
+      <c r="D7" s="17"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -681,10 +721,10 @@
       <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="13">
         <v>1</v>
       </c>
-      <c r="D8" s="14"/>
+      <c r="D8" s="17"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -692,10 +732,10 @@
       <c r="B9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="13">
         <v>1.5</v>
       </c>
-      <c r="D9" s="14"/>
+      <c r="D9" s="17"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -703,305 +743,377 @@
         <v>43593</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="19"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="13">
         <v>3</v>
       </c>
-      <c r="D11" s="14"/>
+      <c r="D11" s="17"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="13">
         <v>0.5</v>
       </c>
-      <c r="D12" s="14"/>
+      <c r="D12" s="17"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="13">
         <v>0.5</v>
       </c>
-      <c r="D13" s="14"/>
+      <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="13">
         <v>0.5</v>
       </c>
-      <c r="D14" s="14"/>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="13">
         <v>0.5</v>
       </c>
-      <c r="D15" s="14"/>
+      <c r="D15" s="17"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="13">
         <v>1</v>
       </c>
-      <c r="D16" s="14"/>
+      <c r="D16" s="17"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>43594</v>
       </c>
       <c r="B17" s="11"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="14"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="17"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="13">
         <v>2</v>
       </c>
-      <c r="D18" s="14"/>
+      <c r="D18" s="17"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="16">
+        <v>34</v>
+      </c>
+      <c r="C19" s="13">
         <v>0.5</v>
       </c>
-      <c r="D19" s="14"/>
+      <c r="D19" s="17"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="16">
+        <v>21</v>
+      </c>
+      <c r="C20" s="13">
         <v>4</v>
       </c>
-      <c r="D20" s="14"/>
+      <c r="D20" s="17"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>43595</v>
       </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="14"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="17"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="16">
+        <v>19</v>
+      </c>
+      <c r="C22" s="13">
         <v>0.5</v>
       </c>
-      <c r="D22" s="14"/>
+      <c r="D22" s="17"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="16">
+        <v>20</v>
+      </c>
+      <c r="C23" s="13">
         <v>1</v>
       </c>
-      <c r="D23" s="14"/>
+      <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="16">
+        <v>22</v>
+      </c>
+      <c r="C24" s="13">
         <v>2</v>
       </c>
-      <c r="D24" s="14"/>
+      <c r="D24" s="17"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>43599</v>
       </c>
       <c r="B25" s="11"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="14"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="17"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="16">
+        <v>23</v>
+      </c>
+      <c r="C26" s="13">
         <v>1</v>
       </c>
-      <c r="D26" s="14"/>
+      <c r="D26" s="17"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="16">
+        <v>24</v>
+      </c>
+      <c r="C27" s="13">
         <v>3</v>
       </c>
-      <c r="D27" s="14"/>
+      <c r="D27" s="17" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="16">
+        <v>25</v>
+      </c>
+      <c r="C28" s="13">
         <v>1</v>
       </c>
-      <c r="D28" s="14"/>
+      <c r="D28" s="17" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="16">
+        <v>27</v>
+      </c>
+      <c r="C29" s="13">
         <v>1</v>
       </c>
-      <c r="D29" s="14"/>
+      <c r="D29" s="17"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="16">
+        <v>28</v>
+      </c>
+      <c r="C30" s="13">
         <v>0.5</v>
       </c>
-      <c r="D30" s="14"/>
+      <c r="D30" s="17"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>43600</v>
       </c>
       <c r="B31" s="11"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="14"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="17"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
-        <v>43601</v>
-      </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="14"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
-        <v>43602</v>
-      </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="14"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="13">
+        <v>3</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="17"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
-        <v>43606</v>
-      </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="14"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="D34" s="17"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>43607</v>
+        <v>43601</v>
       </c>
       <c r="B35" s="11"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="14"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
-        <v>43608</v>
-      </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="14"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
-        <v>43609</v>
-      </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="14"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="7">
-        <v>43613</v>
-      </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="14"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="17"/>
+    </row>
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="13">
+        <v>2</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="13">
+        <v>3</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
-        <v>43614</v>
+        <v>43602</v>
       </c>
       <c r="B39" s="11"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="14"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="17"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
+        <v>43606</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="17"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>43607</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="17"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>43608</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="17"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>43609</v>
+      </c>
+      <c r="B43" s="11"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="17"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <v>43613</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="17"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <v>43614</v>
+      </c>
+      <c r="B45" s="11"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="17"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
         <v>43620</v>
       </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="14"/>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="8">
+      <c r="B46" s="11"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="17"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="8">
         <v>43621</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="15"/>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="B47" s="12"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="18"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="3">
-        <f>SUM(C4:C41)</f>
-        <v>29</v>
+      <c r="C48" s="3">
+        <f>SUM(C4:C47)</f>
+        <v>40.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="79" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented connection status indication
</commit_message>
<xml_diff>
--- a/doc/JournalDeBord.xlsx
+++ b/doc/JournalDeBord.xlsx
@@ -144,7 +144,7 @@
     <t>L'utilisation des subprocess de python a entrainé un certain nombre de contraintes avec lesquelles il a fallut composer</t>
   </si>
   <si>
-    <t xml:space="preserve"> La technique utilisée actuellement, bien que fonctionnelle, entraîne une latence conséquente dans le pilotage. Il est possible que je doive recourir à une librairie externe pour améliorer cela</t>
+    <t xml:space="preserve"> La technique utilisée actuellement, bien que fonctionnelle, entraîne une latence conséquente dans le pilotage. Il est possible que je doive reprendre le fonctionnement de mon code pour rendre la connexion persistante et l'utiliser d'une autre manière mais j'ai malheureusement déjà perdu beaucoup de temps à essayer de faire fonctionner le code tel quel</t>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1016,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="11" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Log view added to GUI
</commit_message>
<xml_diff>
--- a/doc/JournalDeBord.xlsx
+++ b/doc/JournalDeBord.xlsx
@@ -9,9 +9,6 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$C$48</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -22,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Nom, Prénom</t>
   </si>
@@ -132,9 +129,6 @@
     <t>Debug</t>
   </si>
   <si>
-    <t xml:space="preserve">Mon ordinateur plantait lorsque j'essayais de me connecter au wifi avec la clé USB. J'ai donc dû travailler sur mon ordinateur personnel </t>
-  </si>
-  <si>
     <t>Gestion de problème d'infrastructure</t>
   </si>
   <si>
@@ -145,6 +139,18 @@
   </si>
   <si>
     <t xml:space="preserve"> La technique utilisée actuellement, bien que fonctionnelle, entraîne une latence conséquente dans le pilotage. Il est possible que je doive reprendre le fonctionnement de mon code pour rendre la connexion persistante et l'utiliser d'une autre manière mais j'ai malheureusement déjà perdu beaucoup de temps à essayer de faire fonctionner le code tel quel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mon ordinateur plantait lorsque j'essayais de me connecter au wifi avec la clé USB. J'ai donc fini par devoir travailler sur mon ordinateur personnel </t>
+  </si>
+  <si>
+    <t>Résolution du problème de clé Wifi USB</t>
+  </si>
+  <si>
+    <t>Implémentation de la vue de log + remaniement de l'interface</t>
+  </si>
+  <si>
+    <t>L'ergonomie de l'interface n'est pas parfaite mais suffisante pour le moment</t>
   </si>
 </sst>
 </file>
@@ -635,10 +641,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,13 +1001,13 @@
     <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C36" s="13">
         <v>2</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1010,22 +1016,22 @@
         <v>35</v>
       </c>
       <c r="C37" s="13">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" s="13">
         <v>1.5</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1036,33 +1042,41 @@
       <c r="C39" s="13"/>
       <c r="D39" s="17"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="7">
-        <v>43606</v>
-      </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="17"/>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="13">
+        <v>1</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="7">
-        <v>43607</v>
-      </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="13"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="13">
+        <v>0.5</v>
+      </c>
       <c r="D41" s="17"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="7">
-        <v>43608</v>
-      </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="13"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="13">
+        <v>2.5</v>
+      </c>
       <c r="D42" s="17"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
-        <v>43609</v>
+        <v>43606</v>
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="13"/>
@@ -1070,7 +1084,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
-        <v>43613</v>
+        <v>43607</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="13"/>
@@ -1078,7 +1092,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
-        <v>43614</v>
+        <v>43608</v>
       </c>
       <c r="B45" s="11"/>
       <c r="C45" s="13"/>
@@ -1086,34 +1100,58 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
-        <v>43620</v>
+        <v>43609</v>
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="13"/>
       <c r="D46" s="17"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="8">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>43613</v>
+      </c>
+      <c r="B47" s="11"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="17"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>43614</v>
+      </c>
+      <c r="B48" s="11"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="17"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>43620</v>
+      </c>
+      <c r="B49" s="11"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="17"/>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="8">
         <v>43621</v>
       </c>
-      <c r="B47" s="12"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="18"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="B50" s="12"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="18"/>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="3">
-        <f>SUM(C4:C47)</f>
-        <v>40.5</v>
+      <c r="C51" s="3">
+        <f>SUM(C4:C50)</f>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="90" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Files modif and log, settings and key piloting implementation
</commit_message>
<xml_diff>
--- a/doc/JournalDeBord.xlsx
+++ b/doc/JournalDeBord.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Nom, Prénom</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Implémentation du contrôle par l'interface graphique</t>
   </si>
   <si>
-    <t>L'utilisation des subprocess de python a entrainé un certain nombre de contraintes avec lesquelles il a fallut composer</t>
-  </si>
-  <si>
     <t xml:space="preserve"> La technique utilisée actuellement, bien que fonctionnelle, entraîne une latence conséquente dans le pilotage. Il est possible que je doive reprendre le fonctionnement de mon code pour rendre la connexion persistante et l'utiliser d'une autre manière mais j'ai malheureusement déjà perdu beaucoup de temps à essayer de faire fonctionner le code tel quel</t>
   </si>
   <si>
@@ -151,6 +148,18 @@
   </si>
   <si>
     <t>L'ergonomie de l'interface n'est pas parfaite mais suffisante pour le moment</t>
+  </si>
+  <si>
+    <t>Implémentation de la classe SettingSaver</t>
+  </si>
+  <si>
+    <t>Implémentation de la classe NetCamera et Logger</t>
+  </si>
+  <si>
+    <t>Implémentation des méthodes de la classe App</t>
+  </si>
+  <si>
+    <t>L'utilisation des subprocess de python a entrainé un certain nombre de contraintes avec lesquelles il a fallu composer</t>
   </si>
 </sst>
 </file>
@@ -641,10 +650,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1016,7 @@
         <v>2</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1019,7 +1028,7 @@
         <v>3.5</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -1031,7 +1040,7 @@
         <v>1.5</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1045,19 +1054,19 @@
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="13">
         <v>1</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C41" s="13">
         <v>0.5</v>
@@ -1083,40 +1092,52 @@
       <c r="D43" s="17"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="7">
-        <v>43607</v>
-      </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="17"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="7">
-        <v>43608</v>
-      </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="17"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="13">
+        <v>1</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="7">
-        <v>43609</v>
-      </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="17"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="7">
-        <v>43613</v>
-      </c>
-      <c r="B47" s="11"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="C47" s="13"/>
       <c r="D47" s="17"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
-        <v>43614</v>
+        <v>43607</v>
       </c>
       <c r="B48" s="11"/>
       <c r="C48" s="13"/>
@@ -1124,30 +1145,62 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>43620</v>
+        <v>43608</v>
       </c>
       <c r="B49" s="11"/>
       <c r="C49" s="13"/>
       <c r="D49" s="17"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="8">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>43609</v>
+      </c>
+      <c r="B50" s="11"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="17"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <v>43613</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="17"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>43614</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="17"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <v>43620</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="17"/>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="8">
         <v>43621</v>
       </c>
-      <c r="B50" s="12"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="18"/>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="B54" s="12"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="18"/>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C51" s="3">
-        <f>SUM(C4:C50)</f>
-        <v>45</v>
+      <c r="C55" s="3">
+        <f>SUM(C4:C54)</f>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First complete (but unoptimised) version
</commit_message>
<xml_diff>
--- a/doc/JournalDeBord.xlsx
+++ b/doc/JournalDeBord.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>Nom, Prénom</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>implémentation de l'auto-configuration de l'app</t>
+  </si>
+  <si>
+    <t>Création du script de prise de vue pour le raspberry</t>
+  </si>
+  <si>
+    <t>Commentaire du code</t>
+  </si>
+  <si>
+    <t>Problème de compatibilité relatifs aux formats d'image</t>
   </si>
 </sst>
 </file>
@@ -332,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -370,6 +379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,10 +663,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,7 +992,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="11" t="s">
         <v>33</v>
@@ -992,7 +1002,7 @@
       </c>
       <c r="D33" s="17"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="11" t="s">
         <v>11</v>
@@ -1002,7 +1012,7 @@
       </c>
       <c r="D34" s="17"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>43601</v>
       </c>
@@ -1010,7 +1020,7 @@
       <c r="C35" s="13"/>
       <c r="D35" s="17"/>
     </row>
-    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="11" t="s">
         <v>36</v>
@@ -1022,7 +1032,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="11" t="s">
         <v>35</v>
@@ -1034,7 +1044,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="11" t="s">
         <v>37</v>
@@ -1046,7 +1056,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>43602</v>
       </c>
@@ -1054,7 +1064,7 @@
       <c r="C39" s="13"/>
       <c r="D39" s="17"/>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="11" t="s">
         <v>41</v>
@@ -1066,7 +1076,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="11" t="s">
         <v>40</v>
@@ -1076,7 +1086,7 @@
       </c>
       <c r="D41" s="17"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="11" t="s">
         <v>11</v>
@@ -1086,15 +1096,16 @@
       </c>
       <c r="D42" s="17"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>43606</v>
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="13"/>
       <c r="D43" s="17"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F43" s="19"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="11" t="s">
         <v>43</v>
@@ -1106,7 +1117,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="11" t="s">
         <v>44</v>
@@ -1118,7 +1129,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="11" t="s">
         <v>45</v>
@@ -1130,7 +1141,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="11" t="s">
         <v>35</v>
@@ -1140,7 +1151,7 @@
       </c>
       <c r="D47" s="17"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="11" t="s">
         <v>47</v>
@@ -1159,63 +1170,127 @@
       <c r="D49" s="17"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
-        <v>43608</v>
-      </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="13"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="13">
+        <v>1.5</v>
+      </c>
       <c r="D50" s="17"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="7">
-        <v>43609</v>
-      </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="13"/>
+      <c r="A51" s="7"/>
+      <c r="B51" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" s="13">
+        <v>2</v>
+      </c>
       <c r="D51" s="17"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
-        <v>43613</v>
-      </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="13"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="13">
+        <v>1.5</v>
+      </c>
       <c r="D52" s="17"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
-        <v>43614</v>
+        <v>43608</v>
       </c>
       <c r="B53" s="11"/>
       <c r="C53" s="13"/>
       <c r="D53" s="17"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="7">
+      <c r="A54" s="7"/>
+      <c r="B54" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C54" s="13">
+        <v>4</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="D55" s="17"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
+        <v>43609</v>
+      </c>
+      <c r="B56" s="11"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="17"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="7"/>
+      <c r="B57" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="13">
+        <v>4</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
+        <v>43613</v>
+      </c>
+      <c r="B58" s="11"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="17"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
+        <v>43614</v>
+      </c>
+      <c r="B59" s="11"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="17"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
         <v>43620</v>
       </c>
-      <c r="B54" s="11"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="17"/>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="8">
+      <c r="B60" s="11"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="17"/>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="8">
         <v>43621</v>
       </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="18"/>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="B61" s="12"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="18"/>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>1</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C56" s="3">
-        <f>SUM(C4:C55)</f>
-        <v>52</v>
+      <c r="C62" s="3">
+        <f>SUM(C4:C61)</f>
+        <v>67.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Logs and connection feedback adjustment
</commit_message>
<xml_diff>
--- a/doc/JournalDeBord.xlsx
+++ b/doc/JournalDeBord.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>Nom, Prénom</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>Problème de compatibilité relatifs aux formats d'image</t>
+  </si>
+  <si>
+    <t>Première version fonctionnelle</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -663,10 +669,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,39 +1264,59 @@
       <c r="D58" s="17"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="7">
-        <v>43614</v>
-      </c>
-      <c r="B59" s="11"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="17"/>
+      <c r="A59" s="7"/>
+      <c r="B59" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C59" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="7">
-        <v>43620</v>
-      </c>
-      <c r="B60" s="11"/>
+      <c r="A60" s="7"/>
+      <c r="B60" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="C60" s="13"/>
       <c r="D60" s="17"/>
     </row>
-    <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="8">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
+        <v>43614</v>
+      </c>
+      <c r="B61" s="11"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="17"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
+        <v>43620</v>
+      </c>
+      <c r="B62" s="11"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="17"/>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="8">
         <v>43621</v>
       </c>
-      <c r="B61" s="12"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="18"/>
-    </row>
-    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="B63" s="12"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="18"/>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>1</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="3">
-        <f>SUM(C4:C61)</f>
-        <v>67.5</v>
+      <c r="C64" s="3">
+        <f>SUM(C4:C63)</f>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>